<commit_message>
BI_dashboard, log and df generator
</commit_message>
<xml_diff>
--- a/new_graph_build/DL04_annotation.xlsx
+++ b/new_graph_build/DL04_annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\weiping\dev\DCTA\rasa\new_graph_build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18FA43B-5AEB-416B-B518-AA8855C9F5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEEFD2F-FEE8-40F5-B8CF-635B8E9A8981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{12DD387A-0EB2-477F-ABE0-AE22849739F4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12DD387A-0EB2-477F-ABE0-AE22849739F4}"/>
   </bookViews>
   <sheets>
     <sheet name="DL04" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <author>tc={B30F8598-9F9D-45CA-92BE-FAA3C06EBD72}</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{F2DB4546-0DB7-48DA-AEA1-E6C1F0941779}">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{F2DB4546-0DB7-48DA-AEA1-E6C1F0941779}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="1" shapeId="0" xr:uid="{7F8AEF3B-D814-49B0-9B29-F07A0EE8715A}">
+    <comment ref="F10" authorId="1" shapeId="0" xr:uid="{7F8AEF3B-D814-49B0-9B29-F07A0EE8715A}">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="2" shapeId="0" xr:uid="{238F4BC9-A4B4-4507-8E8E-2B43E94D88BC}">
+    <comment ref="F12" authorId="2" shapeId="0" xr:uid="{238F4BC9-A4B4-4507-8E8E-2B43E94D88BC}">
       <text>
         <r>
           <rPr>
@@ -111,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="3" shapeId="0" xr:uid="{55937A4E-90BA-4DC7-89A1-17FD8A5024B3}">
+    <comment ref="F13" authorId="3" shapeId="0" xr:uid="{55937A4E-90BA-4DC7-89A1-17FD8A5024B3}">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="4" shapeId="0" xr:uid="{37EDB3A7-15D6-42AB-BAEC-FAC70DD948CF}">
+    <comment ref="F14" authorId="4" shapeId="0" xr:uid="{37EDB3A7-15D6-42AB-BAEC-FAC70DD948CF}">
       <text>
         <r>
           <rPr>
@@ -151,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="5" shapeId="0" xr:uid="{BB314F63-F3C1-48BE-9283-8BC20EF47F18}">
+    <comment ref="F16" authorId="5" shapeId="0" xr:uid="{BB314F63-F3C1-48BE-9283-8BC20EF47F18}">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="6" shapeId="0" xr:uid="{0277A361-D90E-4E90-8337-2AD0198C5CFE}">
+    <comment ref="F17" authorId="6" shapeId="0" xr:uid="{0277A361-D90E-4E90-8337-2AD0198C5CFE}">
       <text>
         <r>
           <rPr>
@@ -205,7 +205,7 @@
     <author>tc={B30F8598-9F9D-45CA-92BE-FAA3C06EBD72}</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{2DDFAA64-1A7E-4A31-92A9-7DB1FF8B5FAE}">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{2DDFAA64-1A7E-4A31-92A9-7DB1FF8B5FAE}">
       <text>
         <r>
           <rPr>
@@ -226,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="1" shapeId="0" xr:uid="{00B231AA-988E-4E5B-B143-6C966FB78529}">
+    <comment ref="F10" authorId="1" shapeId="0" xr:uid="{00B231AA-988E-4E5B-B143-6C966FB78529}">
       <text>
         <r>
           <rPr>
@@ -246,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="2" shapeId="0" xr:uid="{444BE450-BD53-4708-A237-FC1C6ADF14DF}">
+    <comment ref="F12" authorId="2" shapeId="0" xr:uid="{444BE450-BD53-4708-A237-FC1C6ADF14DF}">
       <text>
         <r>
           <rPr>
@@ -266,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="3" shapeId="0" xr:uid="{7AAB11EC-3E91-474E-A602-A619F13983CE}">
+    <comment ref="F13" authorId="3" shapeId="0" xr:uid="{7AAB11EC-3E91-474E-A602-A619F13983CE}">
       <text>
         <r>
           <rPr>
@@ -286,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="4" shapeId="0" xr:uid="{C55D5D36-9F68-443B-9F9F-FF5779BED78A}">
+    <comment ref="F14" authorId="4" shapeId="0" xr:uid="{C55D5D36-9F68-443B-9F9F-FF5779BED78A}">
       <text>
         <r>
           <rPr>
@@ -306,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="5" shapeId="0" xr:uid="{D94E047B-15E3-4CF4-A59E-0DDB413E61B8}">
+    <comment ref="F16" authorId="5" shapeId="0" xr:uid="{D94E047B-15E3-4CF4-A59E-0DDB413E61B8}">
       <text>
         <r>
           <rPr>
@@ -324,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="6" shapeId="0" xr:uid="{B30F8598-9F9D-45CA-92BE-FAA3C06EBD72}">
+    <comment ref="F17" authorId="6" shapeId="0" xr:uid="{B30F8598-9F9D-45CA-92BE-FAA3C06EBD72}">
       <text>
         <r>
           <rPr>
@@ -363,7 +363,7 @@
     <author>tc={95C646D3-1371-4077-8A9A-581D8BFBAFD4}</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{76A74239-9CDB-4C35-9C69-C1D80D24F868}">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{76A74239-9CDB-4C35-9C69-C1D80D24F868}">
       <text>
         <r>
           <rPr>
@@ -383,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0" xr:uid="{729E1D74-564E-4F14-9C0C-48B0FA36DB96}">
+    <comment ref="F6" authorId="1" shapeId="0" xr:uid="{729E1D74-564E-4F14-9C0C-48B0FA36DB96}">
       <text>
         <r>
           <rPr>
@@ -403,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="2" shapeId="0" xr:uid="{7DD1A409-3959-440E-9552-83C328E00BB7}">
+    <comment ref="F7" authorId="2" shapeId="0" xr:uid="{7DD1A409-3959-440E-9552-83C328E00BB7}">
       <text>
         <r>
           <rPr>
@@ -423,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="3" shapeId="0" xr:uid="{F373EEC7-6D7E-4215-A90A-A671C07398F9}">
+    <comment ref="F8" authorId="3" shapeId="0" xr:uid="{F373EEC7-6D7E-4215-A90A-A671C07398F9}">
       <text>
         <r>
           <rPr>
@@ -443,7 +443,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="4" shapeId="0" xr:uid="{1F6136E9-2F63-4D62-A999-E10DBAFDC99D}">
+    <comment ref="F11" authorId="4" shapeId="0" xr:uid="{1F6136E9-2F63-4D62-A999-E10DBAFDC99D}">
       <text>
         <r>
           <rPr>
@@ -463,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="5" shapeId="0" xr:uid="{8914D62D-B82A-47EF-9B73-0756A4404A3A}">
+    <comment ref="G12" authorId="5" shapeId="0" xr:uid="{8914D62D-B82A-47EF-9B73-0756A4404A3A}">
       <text>
         <r>
           <rPr>
@@ -481,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="6" shapeId="0" xr:uid="{DF5C9B28-6C3D-4E1E-ABBA-5937DDB58F0E}">
+    <comment ref="G13" authorId="6" shapeId="0" xr:uid="{DF5C9B28-6C3D-4E1E-ABBA-5937DDB58F0E}">
       <text>
         <r>
           <rPr>
@@ -499,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="7" shapeId="0" xr:uid="{C4B5D9F3-2339-4181-85E9-8983D253CFA5}">
+    <comment ref="G14" authorId="7" shapeId="0" xr:uid="{C4B5D9F3-2339-4181-85E9-8983D253CFA5}">
       <text>
         <r>
           <rPr>
@@ -517,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="8" shapeId="0" xr:uid="{9340F271-800C-44D5-8387-5A334DDC107E}">
+    <comment ref="F19" authorId="8" shapeId="0" xr:uid="{9340F271-800C-44D5-8387-5A334DDC107E}">
       <text>
         <r>
           <rPr>
@@ -537,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="9" shapeId="0" xr:uid="{B2D3F8A3-B96F-454C-AA91-5CBC58EF2D0C}">
+    <comment ref="F22" authorId="9" shapeId="0" xr:uid="{B2D3F8A3-B96F-454C-AA91-5CBC58EF2D0C}">
       <text>
         <r>
           <rPr>
@@ -576,7 +576,7 @@
     <author>tc={95C646D3-1371-4077-8A9A-581D8BFBAFD4}</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{F8086B97-CD70-4395-A7AC-D9563B7FB3FB}">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{F8086B97-CD70-4395-A7AC-D9563B7FB3FB}">
       <text>
         <r>
           <rPr>
@@ -596,7 +596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0" xr:uid="{3DEA8B06-651F-4F55-9EF4-8CA2C15C3D8A}">
+    <comment ref="F6" authorId="1" shapeId="0" xr:uid="{3DEA8B06-651F-4F55-9EF4-8CA2C15C3D8A}">
       <text>
         <r>
           <rPr>
@@ -616,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="2" shapeId="0" xr:uid="{7E28A660-431A-4046-9DC9-FCBFDB3FFAEB}">
+    <comment ref="F7" authorId="2" shapeId="0" xr:uid="{7E28A660-431A-4046-9DC9-FCBFDB3FFAEB}">
       <text>
         <r>
           <rPr>
@@ -636,7 +636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="3" shapeId="0" xr:uid="{2AE981EF-31A9-4845-A40A-AF0A99E49738}">
+    <comment ref="F8" authorId="3" shapeId="0" xr:uid="{2AE981EF-31A9-4845-A40A-AF0A99E49738}">
       <text>
         <r>
           <rPr>
@@ -656,7 +656,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="4" shapeId="0" xr:uid="{7C7243EE-F3EA-4F0A-86F2-9E1C3E9B58B8}">
+    <comment ref="F11" authorId="4" shapeId="0" xr:uid="{7C7243EE-F3EA-4F0A-86F2-9E1C3E9B58B8}">
       <text>
         <r>
           <rPr>
@@ -676,7 +676,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="5" shapeId="0" xr:uid="{0D575EF3-3E23-4319-A44C-949E752BD613}">
+    <comment ref="G12" authorId="5" shapeId="0" xr:uid="{0D575EF3-3E23-4319-A44C-949E752BD613}">
       <text>
         <r>
           <rPr>
@@ -694,7 +694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="6" shapeId="0" xr:uid="{04E9B787-A009-4F56-84A2-739C01F9A366}">
+    <comment ref="G13" authorId="6" shapeId="0" xr:uid="{04E9B787-A009-4F56-84A2-739C01F9A366}">
       <text>
         <r>
           <rPr>
@@ -712,7 +712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="7" shapeId="0" xr:uid="{0DA74576-BAA4-4482-B50B-54E866C7FB32}">
+    <comment ref="G14" authorId="7" shapeId="0" xr:uid="{0DA74576-BAA4-4482-B50B-54E866C7FB32}">
       <text>
         <r>
           <rPr>
@@ -730,7 +730,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="8" shapeId="0" xr:uid="{634EC86E-AD91-44C0-9270-3818A0D80FDF}">
+    <comment ref="F19" authorId="8" shapeId="0" xr:uid="{634EC86E-AD91-44C0-9270-3818A0D80FDF}">
       <text>
         <r>
           <rPr>
@@ -750,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="9" shapeId="0" xr:uid="{95C646D3-1371-4077-8A9A-581D8BFBAFD4}">
+    <comment ref="F22" authorId="9" shapeId="0" xr:uid="{95C646D3-1371-4077-8A9A-581D8BFBAFD4}">
       <text>
         <r>
           <rPr>
@@ -956,7 +956,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="547">
   <si>
     <t>DL04</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5246,6 +5246,36 @@
 4、肿瘤组织
 5、病理切片
 6、穿刺</t>
+  </si>
+  <si>
+    <t>分类</t>
+  </si>
+  <si>
+    <t>预筛选</t>
+  </si>
+  <si>
+    <t>知情同意</t>
+  </si>
+  <si>
+    <t>年龄</t>
+  </si>
+  <si>
+    <t>受试者类型和疾病特征</t>
+  </si>
+  <si>
+    <t>生殖方面</t>
+  </si>
+  <si>
+    <t>医学疾病</t>
+  </si>
+  <si>
+    <t>既往治疗/合并治疗</t>
+  </si>
+  <si>
+    <t>既往/合并用药临床研究经验</t>
+  </si>
+  <si>
+    <t>其他排除标准</t>
   </si>
 </sst>
 </file>
@@ -6396,732 +6426,807 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5446482-2E81-4C4F-B1C1-699FA4E43505}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="183" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="77"/>
+    <col min="2" max="2" width="15.109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="183" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="77" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="114.6" customHeight="1">
+    <row r="2" spans="1:8" ht="114.6" customHeight="1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="77">
+      <c r="G2" s="1"/>
+      <c r="H2" s="77">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="114.6" customHeight="1">
+    <row r="3" spans="1:8" ht="114.6" customHeight="1">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="81" t="s">
         <v>452</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="77">
+      <c r="G3" s="1"/>
+      <c r="H3" s="77">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="143.4" customHeight="1">
+    <row r="4" spans="1:8" ht="143.4" customHeight="1">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="77">
+      <c r="H4" s="77">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>470</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="77" t="s">
+        <v>470</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="166.2" customHeight="1">
-      <c r="B6" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="166.2" customHeight="1">
       <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="53.7" customHeight="1">
-      <c r="B7" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="53.7" customHeight="1">
       <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="26.7" customHeight="1">
-      <c r="B8" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="26.7" customHeight="1">
       <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="67.5" customHeight="1">
-      <c r="B9" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="67.5" customHeight="1">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="97.5" customHeight="1">
-      <c r="B10" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="97.5" customHeight="1">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="31.95" customHeight="1">
-      <c r="B11" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="31.95" customHeight="1">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" ht="54" customHeight="1">
-      <c r="B12" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="54" customHeight="1">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" ht="120" customHeight="1">
-      <c r="B13" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="120" customHeight="1">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="94.95" customHeight="1">
-      <c r="B14" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="94.95" customHeight="1">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" ht="71.7" customHeight="1">
-      <c r="B16" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="71.7" customHeight="1">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" ht="188.7" customHeight="1">
-      <c r="B17" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="3:7" ht="188.7" customHeight="1">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" ht="52.5" customHeight="1">
-      <c r="B18" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="3:7" ht="52.5" customHeight="1">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" ht="40.950000000000003" customHeight="1">
-      <c r="B19" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="3:7" ht="40.950000000000003" customHeight="1">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:6" ht="22.5" customHeight="1">
-      <c r="B20" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="3:7" ht="22.5" customHeight="1">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" ht="21.45" customHeight="1">
-      <c r="B21" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="3:7" ht="21.45" customHeight="1">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:6" ht="37.950000000000003" customHeight="1">
-      <c r="B22" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="3:7" ht="37.950000000000003" customHeight="1">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="2:6" ht="28.5" customHeight="1">
-      <c r="B23" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="3:7" ht="28.5" customHeight="1">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="2:6" ht="42" customHeight="1">
-      <c r="B24" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="3:7" ht="42" customHeight="1">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:6" ht="24.45" customHeight="1">
-      <c r="B25" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="3:7" ht="24.45" customHeight="1">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" ht="61.95" customHeight="1">
-      <c r="B26" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="3:7" ht="61.95" customHeight="1">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6" ht="103.95" customHeight="1">
-      <c r="B27" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="3:7" ht="103.95" customHeight="1">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:6" ht="22.2" customHeight="1"/>
-    <row r="29" spans="2:6" ht="23.7" customHeight="1"/>
-    <row r="30" spans="2:6" ht="26.7" customHeight="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="3:7" ht="22.2" customHeight="1"/>
+    <row r="29" spans="3:7" ht="23.7" customHeight="1"/>
+    <row r="30" spans="3:7" ht="26.7" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8FC4D1-FD36-41E1-B9DB-3C57396D89CC}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="77" customWidth="1"/>
-    <col min="2" max="2" width="125.88671875" style="77" customWidth="1"/>
-    <col min="3" max="3" width="52.77734375" style="77" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" style="77" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="77" customWidth="1"/>
-    <col min="6" max="6" width="27.21875" style="77" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="77"/>
+    <col min="2" max="2" width="21.88671875" style="77" customWidth="1"/>
+    <col min="3" max="3" width="125.88671875" style="77" customWidth="1"/>
+    <col min="4" max="4" width="52.77734375" style="77" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" style="77" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="77" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" style="77" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="77" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="F1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="G1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="H1" s="79" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="183.6" customHeight="1">
+    <row r="2" spans="1:8" ht="183.6" customHeight="1">
       <c r="A2" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="77" t="s">
+        <v>538</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="80">
+      <c r="H2" s="80">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="172.2" customHeight="1">
+    <row r="3" spans="1:8" ht="172.2" customHeight="1">
       <c r="A3" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="77" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="80">
+      <c r="G3" s="1"/>
+      <c r="H3" s="80">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="68.7" customHeight="1">
+    <row r="4" spans="1:8" ht="68.7" customHeight="1">
       <c r="A4" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="77" t="s">
+        <v>539</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="G4" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="80">
+      <c r="H4" s="80">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="87.45" customHeight="1">
+    <row r="5" spans="1:8" ht="87.45" customHeight="1">
       <c r="A5" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="77" t="s">
+        <v>539</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="80">
+      <c r="H5" s="80">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.2">
+    <row r="6" spans="1:8" ht="43.2">
       <c r="A6" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="77" t="s">
+        <v>540</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="80">
+      <c r="H6" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="219.75" customHeight="1">
+    <row r="7" spans="1:8" ht="219.75" customHeight="1">
       <c r="A7" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="80">
+      <c r="H7" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="81" customHeight="1">
+    <row r="8" spans="1:8" ht="81" customHeight="1">
       <c r="A8" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="80">
+      <c r="H8" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="96" customHeight="1">
+    <row r="9" spans="1:8" ht="96" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="80">
+      <c r="H9" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="108" customHeight="1">
+    <row r="10" spans="1:8" ht="108" customHeight="1">
       <c r="A10" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="80">
+      <c r="H10" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="97.5" customHeight="1">
+    <row r="11" spans="1:8" ht="97.5" customHeight="1">
       <c r="A11" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="80">
+      <c r="G11" s="1"/>
+      <c r="H11" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="97.2" customHeight="1">
+    <row r="12" spans="1:8" ht="97.2" customHeight="1">
       <c r="A12" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="80">
+      <c r="G12" s="1"/>
+      <c r="H12" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="100.8" customHeight="1">
+    <row r="13" spans="1:8" ht="100.8" customHeight="1">
       <c r="A13" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="G13" s="80">
+      <c r="H13" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="120" customHeight="1">
+    <row r="14" spans="1:8" ht="120" customHeight="1">
       <c r="A14" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="80">
+      <c r="G14" s="1"/>
+      <c r="H14" s="80">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="94.95" customHeight="1">
+    <row r="15" spans="1:8" ht="94.95" customHeight="1">
       <c r="A15" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="80">
+      <c r="H15" s="80">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="80">
+      <c r="H16" s="80">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="153.9" customHeight="1">
+    <row r="17" spans="1:8" ht="153.9" customHeight="1">
       <c r="A17" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="77" t="s">
+        <v>542</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="77" t="s">
+      <c r="G17" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="80">
+      <c r="H17" s="80">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="188.7" customHeight="1">
+    <row r="18" spans="1:8" ht="188.7" customHeight="1">
       <c r="A18" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="77" t="s">
+        <v>542</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="80">
+      <c r="H18" s="80">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="138.9" customHeight="1">
+    <row r="19" spans="1:8" ht="138.9" customHeight="1">
       <c r="A19" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="77" t="s">
+        <v>542</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="D19" s="82" t="s">
         <v>455</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="77" t="s">
+      <c r="G19" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="80">
+      <c r="H19" s="80">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="40.950000000000003" customHeight="1">
-      <c r="B20" s="1"/>
+    <row r="20" spans="1:8" ht="40.950000000000003" customHeight="1">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" ht="22.5" customHeight="1">
-      <c r="B21" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="22.5" customHeight="1">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" ht="21.45" customHeight="1">
-      <c r="B22" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="21.45" customHeight="1">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="37.950000000000003" customHeight="1">
-      <c r="B23" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="37.950000000000003" customHeight="1">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="28.5" customHeight="1">
-      <c r="B24" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="28.5" customHeight="1">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" ht="42" customHeight="1">
-      <c r="B25" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" ht="42" customHeight="1">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="24.45" customHeight="1">
-      <c r="B26" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" ht="24.45" customHeight="1">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="61.95" customHeight="1">
-      <c r="B27" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="61.95" customHeight="1">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" ht="103.95" customHeight="1">
-      <c r="B28" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="103.95" customHeight="1">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" ht="22.2" customHeight="1"/>
-    <row r="30" spans="1:7" ht="23.7" customHeight="1"/>
-    <row r="31" spans="1:7" ht="26.7" customHeight="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="22.2" customHeight="1"/>
+    <row r="30" spans="1:8" ht="23.7" customHeight="1"/>
+    <row r="31" spans="1:8" ht="26.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7131,481 +7236,539 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD63055-07F4-4594-8BE0-194FC94EB51F}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="77.5546875" customWidth="1"/>
-    <col min="3" max="3" width="40.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="77" customWidth="1"/>
+    <col min="3" max="3" width="77.5546875" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>474</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="77" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="H1" s="79" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="114.6" customHeight="1">
+    <row r="2" spans="1:8" ht="114.6" customHeight="1">
       <c r="A2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>538</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="G2" s="80">
+      <c r="H2" s="80">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="172.2" customHeight="1">
+    <row r="3" spans="1:8" ht="172.2" customHeight="1">
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="77" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="80">
+      <c r="G3" s="1"/>
+      <c r="H3" s="80">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="68.7" customHeight="1">
+    <row r="4" spans="1:8" ht="68.7" customHeight="1">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="77" t="s">
+        <v>539</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="G4" s="80">
+      <c r="H4" s="80">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="87.45" customHeight="1">
+    <row r="5" spans="1:8" ht="87.45" customHeight="1">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="77" t="s">
+        <v>539</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="G5" s="80">
+      <c r="H5" s="80">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.2">
+    <row r="6" spans="1:8" ht="43.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="77" t="s">
+        <v>540</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="G6" s="80">
+      <c r="H6" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="219.75" customHeight="1">
+    <row r="7" spans="1:8" ht="219.75" customHeight="1">
       <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>541</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="G7" s="80">
+      <c r="H7" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="136.80000000000001" customHeight="1">
+    <row r="8" spans="1:8" ht="136.80000000000001" customHeight="1">
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="G8" s="80">
+      <c r="H8" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="116.4" customHeight="1">
+    <row r="9" spans="1:8" ht="116.4" customHeight="1">
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="G9" s="80">
+      <c r="H9" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="108" customHeight="1">
+    <row r="10" spans="1:8" ht="108" customHeight="1">
       <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="G10" s="80">
+      <c r="H10" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="97.5" customHeight="1">
+    <row r="11" spans="1:8" ht="97.5" customHeight="1">
       <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="80">
+      <c r="G11" s="1"/>
+      <c r="H11" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="97.2" customHeight="1">
+    <row r="12" spans="1:8" ht="97.2" customHeight="1">
       <c r="A12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="80">
+      <c r="G12" s="1"/>
+      <c r="H12" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="100.8" customHeight="1">
+    <row r="13" spans="1:8" ht="100.8" customHeight="1">
       <c r="A13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="G13" s="80">
+      <c r="H13" s="80">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="120" customHeight="1">
+    <row r="14" spans="1:8" ht="120" customHeight="1">
       <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="80">
+      <c r="G14" s="1"/>
+      <c r="H14" s="80">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="94.95" customHeight="1">
+    <row r="15" spans="1:8" ht="94.95" customHeight="1">
       <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="G15" s="80">
+      <c r="H15" s="80">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="77" t="s">
+        <v>541</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="G16" s="80">
+      <c r="H16" s="80">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="153.9" customHeight="1">
+    <row r="17" spans="1:8" ht="153.9" customHeight="1">
       <c r="A17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>542</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="G17" s="80">
+      <c r="H17" s="80">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="188.7" customHeight="1">
+    <row r="18" spans="1:8" ht="188.7" customHeight="1">
       <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="77" t="s">
+        <v>542</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="G18" s="80">
+      <c r="H18" s="80">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="138.9" customHeight="1">
+    <row r="19" spans="1:8" ht="138.9" customHeight="1">
       <c r="A19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="77" t="s">
+        <v>542</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="D19" s="82" t="s">
         <v>455</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="G19" s="80">
+      <c r="H19" s="80">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="40.950000000000003" customHeight="1">
-      <c r="B20" s="1"/>
+    <row r="20" spans="1:8" ht="40.950000000000003" customHeight="1">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="G20" s="77"/>
-    </row>
-    <row r="21" spans="1:7" ht="22.5" customHeight="1">
-      <c r="B21" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="77"/>
+    </row>
+    <row r="21" spans="1:8" ht="22.5" customHeight="1">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="G21" s="77"/>
-    </row>
-    <row r="22" spans="1:7" ht="21.45" customHeight="1">
-      <c r="B22" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="H21" s="77"/>
+    </row>
+    <row r="22" spans="1:8" ht="21.45" customHeight="1">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="G22" s="77"/>
-    </row>
-    <row r="23" spans="1:7" ht="37.950000000000003" customHeight="1">
-      <c r="B23" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="H22" s="77"/>
+    </row>
+    <row r="23" spans="1:8" ht="37.950000000000003" customHeight="1">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="G23" s="77"/>
-    </row>
-    <row r="24" spans="1:7" ht="28.5" customHeight="1">
-      <c r="B24" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="77"/>
+    </row>
+    <row r="24" spans="1:8" ht="28.5" customHeight="1">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="77"/>
-    </row>
-    <row r="25" spans="1:7" ht="42" customHeight="1">
-      <c r="B25" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="77"/>
+    </row>
+    <row r="25" spans="1:8" ht="42" customHeight="1">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="G25" s="77"/>
-    </row>
-    <row r="26" spans="1:7" ht="24.45" customHeight="1">
-      <c r="B26" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="H25" s="77"/>
+    </row>
+    <row r="26" spans="1:8" ht="24.45" customHeight="1">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="G26" s="77"/>
-    </row>
-    <row r="27" spans="1:7" ht="61.95" customHeight="1">
-      <c r="B27" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="H26" s="77"/>
+    </row>
+    <row r="27" spans="1:8" ht="61.95" customHeight="1">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="77"/>
-    </row>
-    <row r="28" spans="1:7" ht="103.95" customHeight="1">
-      <c r="B28" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="77"/>
+    </row>
+    <row r="28" spans="1:8" ht="103.95" customHeight="1">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="77"/>
-    </row>
-    <row r="29" spans="1:7" ht="22.2" customHeight="1">
-      <c r="G29" s="77"/>
-    </row>
-    <row r="30" spans="1:7" ht="23.7" customHeight="1">
-      <c r="G30" s="77"/>
-    </row>
-    <row r="31" spans="1:7" ht="26.7" customHeight="1">
-      <c r="G31" s="77"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="77"/>
+    </row>
+    <row r="29" spans="1:8" ht="22.2" customHeight="1">
+      <c r="H29" s="77"/>
+    </row>
+    <row r="30" spans="1:8" ht="23.7" customHeight="1">
+      <c r="H30" s="77"/>
+    </row>
+    <row r="31" spans="1:8" ht="26.7" customHeight="1">
+      <c r="H31" s="77"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7617,633 +7780,717 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070E72AF-FF6F-43FC-9531-A153FAD1DDB2}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="77" customWidth="1"/>
-    <col min="2" max="2" width="163.21875" style="77" customWidth="1"/>
-    <col min="3" max="4" width="28.44140625" style="77" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="77" customWidth="1"/>
-    <col min="6" max="6" width="44.44140625" style="77" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="77"/>
+    <col min="1" max="2" width="15.109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="163.21875" style="77" customWidth="1"/>
+    <col min="4" max="5" width="28.44140625" style="77" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="77" customWidth="1"/>
+    <col min="7" max="7" width="44.44140625" style="77" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="77" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="F1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="G1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="78" t="s">
+      <c r="H1" s="78" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="114.6" customHeight="1">
+    <row r="2" spans="1:8" ht="114.6" customHeight="1">
       <c r="A2" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="77">
+      <c r="H2" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="114.6" customHeight="1">
+    <row r="3" spans="1:8" ht="114.6" customHeight="1">
       <c r="A3" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G3" s="77">
+      <c r="H3" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="68.7" customHeight="1">
+    <row r="4" spans="1:8" ht="68.7" customHeight="1">
       <c r="A4" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="G4" s="77">
+      <c r="H4" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="243" customHeight="1">
+    <row r="5" spans="1:8" ht="243" customHeight="1">
       <c r="A5" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="77">
+      <c r="H5" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="201.6">
+    <row r="6" spans="1:8" ht="201.6">
       <c r="A6" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G6" s="77">
+      <c r="H6" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="324.60000000000002" customHeight="1">
+    <row r="7" spans="1:8" ht="324.60000000000002" customHeight="1">
       <c r="A7" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="77">
+      <c r="H7" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="90" customHeight="1">
+    <row r="8" spans="1:8" ht="90" customHeight="1">
       <c r="A8" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="77">
+      <c r="H8" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57.9" customHeight="1">
+    <row r="9" spans="1:8" ht="57.9" customHeight="1">
       <c r="A9" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="77">
+      <c r="H9" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="67.5" customHeight="1">
+    <row r="10" spans="1:8" ht="67.5" customHeight="1">
       <c r="A10" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="77">
+      <c r="H10" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="97.5" customHeight="1">
+    <row r="11" spans="1:8" ht="97.5" customHeight="1">
       <c r="A11" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="77">
+      <c r="H11" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="82.5" customHeight="1">
+    <row r="12" spans="1:8" ht="82.5" customHeight="1">
       <c r="A12" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G12" s="77">
+      <c r="H12" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="84.9" customHeight="1">
+    <row r="13" spans="1:8" ht="84.9" customHeight="1">
       <c r="A13" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="77">
+      <c r="H13" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="234.9" customHeight="1">
+    <row r="14" spans="1:8" ht="234.9" customHeight="1">
       <c r="A14" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G14" s="77">
+      <c r="H14" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="94.95" customHeight="1">
+    <row r="15" spans="1:8" ht="94.95" customHeight="1">
       <c r="A15" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G15" s="77">
+      <c r="H15" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="72">
+    <row r="16" spans="1:8" ht="72">
       <c r="A16" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="G16" s="77">
+      <c r="H16" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="159.9" customHeight="1">
+    <row r="17" spans="1:8" ht="159.9" customHeight="1">
       <c r="A17" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="F17" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="77" t="s">
+      <c r="G17" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="77">
+      <c r="H17" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="221.4" customHeight="1">
+    <row r="18" spans="1:8" ht="221.4" customHeight="1">
       <c r="A18" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="77" t="s">
+        <v>544</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G18" s="77">
+      <c r="H18" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="89.25" customHeight="1">
+    <row r="19" spans="1:8" ht="89.25" customHeight="1">
       <c r="A19" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="77" t="s">
+        <v>544</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G19" s="77">
+      <c r="H19" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="79.5" customHeight="1">
+    <row r="20" spans="1:8" ht="79.5" customHeight="1">
       <c r="A20" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="77" t="s">
+        <v>544</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="77">
+      <c r="H20" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="22.5" customHeight="1">
+    <row r="21" spans="1:8" ht="22.5" customHeight="1">
       <c r="A21" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="F21" s="77" t="s">
+      <c r="G21" s="77" t="s">
         <v>531</v>
       </c>
-      <c r="G21" s="77">
+      <c r="H21" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="48.6" customHeight="1">
+    <row r="22" spans="1:8" ht="48.6" customHeight="1">
       <c r="A22" s="77" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="77" t="s">
+      <c r="G22" s="77" t="s">
         <v>148</v>
       </c>
-      <c r="G22" s="77">
+      <c r="H22" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="37.950000000000003" customHeight="1">
+    <row r="23" spans="1:8" ht="37.950000000000003" customHeight="1">
       <c r="A23" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F23" s="77" t="s">
+      <c r="G23" s="77" t="s">
         <v>530</v>
       </c>
-      <c r="G23" s="77">
+      <c r="H23" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="134.4" customHeight="1">
+    <row r="24" spans="1:8" ht="134.4" customHeight="1">
       <c r="A24" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G24" s="77">
+      <c r="H24" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="42" customHeight="1">
+    <row r="25" spans="1:8" ht="42" customHeight="1">
       <c r="A25" s="77" t="s">
         <v>154</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="77" t="s">
+        <v>546</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F25" s="77" t="s">
+      <c r="G25" s="77" t="s">
         <v>529</v>
       </c>
-      <c r="G25" s="77">
+      <c r="H25" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="56.4" customHeight="1">
+    <row r="26" spans="1:8" ht="56.4" customHeight="1">
       <c r="A26" s="77" t="s">
         <v>157</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="77" t="s">
+        <v>546</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="77" t="s">
+      <c r="F26" s="77" t="s">
         <v>159</v>
       </c>
-      <c r="F26" s="77" t="s">
+      <c r="G26" s="77" t="s">
         <v>160</v>
       </c>
-      <c r="G26" s="77">
+      <c r="H26" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="61.95" customHeight="1">
+    <row r="27" spans="1:8" ht="61.95" customHeight="1">
       <c r="A27" s="77" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="77" t="s">
+        <v>546</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="77">
+      <c r="H27" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="103.95" customHeight="1">
+    <row r="28" spans="1:8" ht="103.95" customHeight="1">
       <c r="A28" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="77" t="s">
+        <v>546</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="G28" s="77">
+      <c r="H28" s="77">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="22.2" customHeight="1"/>
-    <row r="30" spans="1:7" ht="23.7" customHeight="1"/>
-    <row r="31" spans="1:7" ht="26.7" customHeight="1"/>
+    <row r="29" spans="1:8" ht="22.2" customHeight="1"/>
+    <row r="30" spans="1:8" ht="23.7" customHeight="1"/>
+    <row r="31" spans="1:8" ht="26.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8253,634 +8500,719 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D784C70D-BB82-4D43-8C41-8A16CD8E3231}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="77"/>
+    <col min="2" max="2" width="15.109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="77" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="78" t="s">
+      <c r="H1" s="78" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="114.6" customHeight="1">
+    <row r="2" spans="1:8" ht="114.6" customHeight="1">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="G2" s="77">
+      <c r="H2" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="114.6" customHeight="1">
+    <row r="3" spans="1:8" ht="114.6" customHeight="1">
       <c r="A3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="G3" s="77">
+      <c r="H3" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="68.7" customHeight="1">
+    <row r="4" spans="1:8" ht="68.7" customHeight="1">
       <c r="A4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="G4" s="77">
+      <c r="H4" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="243" customHeight="1">
+    <row r="5" spans="1:8" ht="243" customHeight="1">
       <c r="A5" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="G5" s="77">
+      <c r="H5" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="201.6">
+    <row r="6" spans="1:8" ht="201.6">
       <c r="A6" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="G6" s="77">
+      <c r="H6" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="324.60000000000002" customHeight="1">
+    <row r="7" spans="1:8" ht="324.60000000000002" customHeight="1">
       <c r="A7" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="G7" s="77">
+      <c r="H7" s="77">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="90" customHeight="1">
+    <row r="8" spans="1:8" ht="90" customHeight="1">
       <c r="A8" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="G8" s="77">
+      <c r="H8" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57.9" customHeight="1">
+    <row r="9" spans="1:8" ht="57.9" customHeight="1">
       <c r="A9" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="77">
+      <c r="H9" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="67.5" customHeight="1">
+    <row r="10" spans="1:8" ht="67.5" customHeight="1">
       <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="77">
+      <c r="H10" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="97.5" customHeight="1">
+    <row r="11" spans="1:8" ht="97.5" customHeight="1">
       <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="G11" s="77">
+      <c r="H11" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="82.5" customHeight="1">
+    <row r="12" spans="1:8" ht="82.5" customHeight="1">
       <c r="A12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="G12" s="77">
+      <c r="H12" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="84.9" customHeight="1">
+    <row r="13" spans="1:8" ht="84.9" customHeight="1">
       <c r="A13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="77">
+      <c r="H13" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="234.9" customHeight="1">
+    <row r="14" spans="1:8" ht="234.9" customHeight="1">
       <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="G14" s="77">
+      <c r="H14" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="94.95" customHeight="1">
+    <row r="15" spans="1:8" ht="94.95" customHeight="1">
       <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="G15" s="77">
+      <c r="H15" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="100.8">
+    <row r="16" spans="1:8" ht="100.8">
       <c r="A16" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="77">
+      <c r="H16" s="77">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="159.9" customHeight="1">
+    <row r="17" spans="1:8" ht="159.9" customHeight="1">
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="77" t="s">
+        <v>543</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>132</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="77">
+      <c r="H17" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="221.4" customHeight="1">
+    <row r="18" spans="1:8" ht="221.4" customHeight="1">
       <c r="A18" t="s">
         <v>134</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>544</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="G18" s="77">
+      <c r="H18" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="89.25" customHeight="1">
+    <row r="19" spans="1:8" ht="89.25" customHeight="1">
       <c r="A19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="77" t="s">
+        <v>544</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G19" s="77">
+      <c r="H19" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="79.5" customHeight="1">
+    <row r="20" spans="1:8" ht="79.5" customHeight="1">
       <c r="A20" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="77" t="s">
+        <v>544</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="77">
+      <c r="H20" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="22.5" customHeight="1">
+    <row r="21" spans="1:8" ht="22.5" customHeight="1">
       <c r="A21" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>545</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>483</v>
       </c>
-      <c r="G21" s="77">
+      <c r="H21" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="21.45" customHeight="1">
+    <row r="22" spans="1:8" ht="21.45" customHeight="1">
       <c r="A22" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>484</v>
       </c>
-      <c r="G22" s="77">
+      <c r="H22" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="37.950000000000003" customHeight="1">
+    <row r="23" spans="1:8" ht="37.950000000000003" customHeight="1">
       <c r="A23" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>485</v>
       </c>
-      <c r="G23" s="77">
+      <c r="H23" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="134.4" customHeight="1">
+    <row r="24" spans="1:8" ht="134.4" customHeight="1">
       <c r="A24" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="77" t="s">
+        <v>545</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G24" s="77">
+      <c r="H24" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="42" customHeight="1">
+    <row r="25" spans="1:8" ht="42" customHeight="1">
       <c r="A25" t="s">
         <v>154</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>546</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>486</v>
       </c>
-      <c r="G25" s="77">
+      <c r="H25" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="56.4" customHeight="1">
+    <row r="26" spans="1:8" ht="56.4" customHeight="1">
       <c r="A26" t="s">
         <v>157</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="77" t="s">
+        <v>546</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>159</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>487</v>
       </c>
-      <c r="G26" s="77">
+      <c r="H26" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="61.95" customHeight="1">
+    <row r="27" spans="1:8" ht="61.95" customHeight="1">
       <c r="A27" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="77" t="s">
+        <v>546</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="77">
+      <c r="H27" s="77">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="103.95" customHeight="1">
+    <row r="28" spans="1:8" ht="103.95" customHeight="1">
       <c r="A28" t="s">
         <v>165</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="77" t="s">
+        <v>546</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="G28" s="77">
+      <c r="H28" s="77">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="22.2" customHeight="1"/>
-    <row r="30" spans="1:7" ht="23.7" customHeight="1"/>
-    <row r="31" spans="1:7" ht="26.7" customHeight="1"/>
+    <row r="29" spans="1:8" ht="22.2" customHeight="1"/>
+    <row r="30" spans="1:8" ht="23.7" customHeight="1"/>
+    <row r="31" spans="1:8" ht="26.7" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12027,21 +12359,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099F474F600D05146912A548CFFB3B3DE" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd1e41a35726873ac6091597d8bfca82">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="060f33fb-d6f8-41d3-bc35-c7620efd4ad0" xmlns:ns3="240bb027-5beb-4c51-8c68-3e71576f565c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e32dd6ec86430cdd980600f8bc57aae4" ns2:_="" ns3:_="">
     <xsd:import namespace="060f33fb-d6f8-41d3-bc35-c7620efd4ad0"/>
@@ -12206,24 +12523,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFABE7C6-D1B3-4CD5-A6EF-ED1B84B759D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B63F4C5-93C2-4082-B8DD-25012DD4CFEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70ABE67E-D87E-479A-B257-FE11B75E67E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12240,4 +12555,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFABE7C6-D1B3-4CD5-A6EF-ED1B84B759D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B63F4C5-93C2-4082-B8DD-25012DD4CFEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>